<commit_message>
updated combined template, combined publication measures
</commit_message>
<xml_diff>
--- a/StateOfPractice/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
   <si>
     <t xml:space="preserve">Metrics &amp; Description</t>
   </si>
@@ -112,10 +112,10 @@
     <t xml:space="preserve">({open source, freeware, commercial, unclear})</t>
   </si>
   <si>
-    <t xml:space="preserve">Publications using the software? Refers to publications that have used the software in their research.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publications about the software? Refers to publications that have only mentioned the software and have not clearly applied it.</t>
+    <t xml:space="preserve">Publications about the software? Refers to publications that have used or mentioned the software.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(number or {unknown})</t>
   </si>
   <si>
     <t xml:space="preserve">Source code URL?</t>
@@ -634,15 +634,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ120"/>
+  <dimension ref="A1:AMJ119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -784,382 +784,380 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>31</v>
+      </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="46.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="46.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+    <row r="20" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="75.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="21" customFormat="false" ht="75.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" s="6" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" s="6" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="AMJ23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="B22" s="5"/>
+      <c r="AMJ22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
         <v>52</v>
       </c>
+      <c r="B31" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B32" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>58</v>
+      <c r="A36" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="38" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="AMJ40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="5"/>
+      <c r="AMJ39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="73.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="73.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="8" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="AMJ50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="AMJ51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+    <row r="57" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="AMJ59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="56.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="5"/>
+      <c r="AMJ58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="56.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
+    <row r="62" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="AMJ64" s="0"/>
+      <c r="B63" s="5"/>
+      <c r="AMJ63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>41</v>
@@ -1167,183 +1165,183 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>91</v>
+    <row r="67" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
-        <v>92</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="AMJ70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="46.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+    <row r="79" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="AMJ71" s="0"/>
-    </row>
-    <row r="72" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B72" s="8" t="s">
+    </row>
+    <row r="80" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="AMJ80" s="0"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="46.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="AMJ81" s="0"/>
+      <c r="C81" s="10"/>
+      <c r="E81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="10"/>
-      <c r="E82" s="9"/>
+        <v>107</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
-        <v>107</v>
+      <c r="A83" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" s="6" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="AMJ85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" s="6" customFormat="true" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="AMJ86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>87</v>
@@ -1351,15 +1349,15 @@
     </row>
     <row r="90" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>87</v>
@@ -1367,7 +1365,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>87</v>
@@ -1375,7 +1373,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>87</v>
@@ -1383,51 +1381,51 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
+    <row r="95" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="97" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4" t="s">
+    <row r="96" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B97" s="5"/>
-      <c r="AMJ97" s="0"/>
+      <c r="B96" s="5"/>
+      <c r="AMJ96" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>37</v>
@@ -1435,36 +1433,36 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
+    <row r="102" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B103" s="2"/>
-    </row>
-    <row r="106" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="4" t="s">
+      <c r="B102" s="2"/>
+    </row>
+    <row r="105" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B106" s="5"/>
-      <c r="AMJ106" s="0"/>
+      <c r="B105" s="5"/>
+      <c r="AMJ105" s="0"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>12</v>
@@ -1472,7 +1470,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>12</v>
@@ -1480,7 +1478,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>12</v>
@@ -1488,7 +1486,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>12</v>
@@ -1496,46 +1494,46 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="35.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="115" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="4" t="s">
+    <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B115" s="5"/>
-      <c r="AMJ115" s="0"/>
+      <c r="B114" s="5"/>
+      <c r="AMJ114" s="0"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>12</v>
@@ -1543,7 +1541,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>12</v>
@@ -1551,7 +1549,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>12</v>
@@ -1559,17 +1557,9 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B120" s="8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>